<commit_message>
Automatisk commit och push av repositoryt till github 01 nov 2024 kl. 15:14
</commit_message>
<xml_diff>
--- a/NApendling.xlsx
+++ b/NApendling.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">regionkod</t>
   </si>
@@ -20,25 +20,34 @@
     <t xml:space="preserve">region</t>
   </si>
   <si>
+    <t xml:space="preserve">utbildning</t>
+  </si>
+  <si>
     <t xml:space="preserve">kön</t>
   </si>
   <si>
     <t xml:space="preserve">år</t>
   </si>
   <si>
-    <t xml:space="preserve">pendlingstyp</t>
+    <t xml:space="preserve">variabel</t>
   </si>
   <si>
     <t xml:space="preserve">andel</t>
   </si>
   <si>
-    <t xml:space="preserve">2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vansbro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">män och kvinnor</t>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stockholms län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samtliga utbildningsgrupper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022</t>
   </si>
   <si>
     <t xml:space="preserve">Andel utpendling</t>
@@ -47,88 +56,124 @@
     <t xml:space="preserve">Andel inpendling</t>
   </si>
   <si>
-    <t xml:space="preserve">2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malung-Sälen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gagnef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leksand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rättvik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orsa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Älvdalen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smedjebacken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borlänge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Säter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedemora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avesta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ludvika</t>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uppsala län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Södermanlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Östergötlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jönköpings län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kronobergs län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalmar län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gotlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blekinge län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skåne län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hallands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Västra Götalands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Värmlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Örebro län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Västmanlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalarnas län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gävleborgs län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Västernorrlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jämtlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Västerbottens län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norrbottens län</t>
   </si>
 </sst>
 </file>
@@ -479,605 +524,974 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="n">
-        <v>17.0193192272309</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.86110378271084</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="n">
-        <v>14.3399810066477</v>
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9.1825843963394</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="n">
-        <v>12.5535227715064</v>
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="n">
+        <v>25.6418398871869</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="n">
-        <v>14.5655067503328</v>
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="n">
+        <v>13.4200680591852</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="n">
-        <v>54.5004945598417</v>
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20.6521232823539</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="n">
-        <v>27.7411247251021</v>
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10.4342111028349</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="n">
-        <v>29.9595669753489</v>
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6.4208485852208</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="n">
-        <v>24.5680573114201</v>
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5.23484624693876</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="n">
-        <v>35.4554170661553</v>
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6.5235859074498</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="n">
-        <v>20.5757432751298</v>
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7.46580702430592</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="n">
-        <v>47.0283450167632</v>
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.51192972388373</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="n">
-        <v>26.3559322033898</v>
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="n">
+        <v>12.7486475677269</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="n">
-        <v>21.1914641375222</v>
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>7.63566362336582</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" t="n">
-        <v>14.7483167681949</v>
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4.93045803435739</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" t="n">
-        <v>51.3022410660206</v>
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7.27827824054879</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" t="n">
-        <v>25.3712871287129</v>
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3.88747802305138</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" t="n">
-        <v>17.4344436569809</v>
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="n">
+        <v>12.076793926564</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" t="n">
-        <v>25.7015306122449</v>
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9.50033811706364</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" t="n">
-        <v>24.3440233236152</v>
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.16138596991301</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="n">
-        <v>24.9268341911394</v>
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3.6579783621392</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="n">
-        <v>24.8882450331126</v>
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="n">
+        <v>23.2377017629398</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="n">
-        <v>37.5253898853582</v>
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="n">
+        <v>11.3811925552321</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" t="n">
-        <v>55.5131004366812</v>
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5.06875312459047</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" t="n">
-        <v>32.5703254274683</v>
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="n">
+        <v>6.03417109569708</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" t="n">
-        <v>33.1485429992893</v>
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="n">
+        <v>8.45495762508211</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" t="n">
-        <v>29.2569193742479</v>
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="n">
+        <v>4.69109650732228</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" t="n">
-        <v>22.65495363592</v>
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7.62700140526136</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" t="n">
-        <v>23.9028137904542</v>
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="n">
+        <v>7.99344395451381</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" t="n">
-        <v>18.1857676600921</v>
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="n">
+        <v>15.4772997461684</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" t="n">
-        <v>24.3330118932819</v>
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="n">
+        <v>11.0352057898475</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="n">
+        <v>6.93083550454756</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5.55325758128746</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="n">
+        <v>8.13279947150902</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6.11559361106537</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="n">
+        <v>5.34431809680557</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" t="n">
+        <v>4.61287647480116</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="n">
+        <v>7.10524583689857</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" t="n">
+        <v>4.50947225981055</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="n">
+        <v>4.63645286428716</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3.79864210724838</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="n">
+        <v>4.11866384718652</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3.35290892045354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diverse uppdateringar av text
</commit_message>
<xml_diff>
--- a/NApendling.xlsx
+++ b/NApendling.xlsx
@@ -12,123 +12,168 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+  <si>
+    <t xml:space="preserve">regionkod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utbildning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kön</t>
+  </si>
   <si>
     <t xml:space="preserve">år</t>
   </si>
   <si>
-    <t xml:space="preserve">regionkod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kön</t>
-  </si>
-  <si>
     <t xml:space="preserve">variabel</t>
   </si>
   <si>
     <t xml:space="preserve">andel</t>
   </si>
   <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stockholms län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samtliga utbildningsgrupper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalt</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023</t>
   </si>
   <si>
-    <t xml:space="preserve">2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vansbro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">män och kvinnor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Andel utpendling</t>
   </si>
   <si>
     <t xml:space="preserve">Andel inpendling</t>
   </si>
   <si>
-    <t xml:space="preserve">Malung-Sälen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gagnef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leksand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rättvik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orsa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Älvdalen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smedjebacken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borlänge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Säter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedemora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avesta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ludvika</t>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uppsala län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Södermanlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Östergötlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jönköpings län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kronobergs län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalmar län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gotlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blekinge län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skåne län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hallands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Västra Götalands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Värmlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Örebro län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Västmanlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalarnas län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gävleborgs län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Västernorrlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jämtlands län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Västerbottens län</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norrbottens län</t>
   </si>
 </sst>
 </file>
@@ -479,605 +524,974 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
-        <v>17.5180288461538</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.85673440229401</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="n">
-        <v>10.7317073170732</v>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9.21976169736383</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="n">
-        <v>13.1748664086973</v>
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="n">
+        <v>25.7688358806037</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="n">
-        <v>13.6680102601686</v>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="n">
+        <v>13.4002767934165</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="n">
-        <v>53.422765831525</v>
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20.5469143943214</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="n">
-        <v>26.4485981308411</v>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10.2603194630637</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="n">
-        <v>29.4632513837045</v>
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6.32514326379265</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" t="n">
-        <v>24.6424642464246</v>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5.1690143515271</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="n">
-        <v>35.608082348456</v>
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6.54216111972173</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" t="n">
-        <v>21.8598195697432</v>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7.2701019551679</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="n">
-        <v>48.234255444379</v>
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.27135077699562</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" t="n">
-        <v>25.4661016949153</v>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="n">
+        <v>12.7346818435489</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="n">
-        <v>22.6114649681529</v>
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>7.7064581827738</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
       </c>
-      <c r="F15" t="n">
-        <v>15.5183312262958</v>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5.12229244054224</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" t="n">
-        <v>51.8366549433372</v>
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7.50716764750264</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
       </c>
-      <c r="F17" t="n">
-        <v>26.6587325200833</v>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3.99404808520636</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" t="n">
-        <v>17.9346225581624</v>
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="n">
+        <v>12.37411535611</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
-      <c r="F19" t="n">
-        <v>26.1092451829592</v>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9.48964274992495</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" t="n">
-        <v>23.9265022347293</v>
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.38304973117428</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
       </c>
-      <c r="F21" t="n">
-        <v>25.3549036806029</v>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3.68878908410821</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="n">
-        <v>25.4136546184739</v>
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="n">
+        <v>23.2553077060978</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
       </c>
-      <c r="F23" t="n">
-        <v>36.5926937521338</v>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="n">
+        <v>11.4327725193773</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="n">
-        <v>55.8351177730193</v>
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5.07913986213608</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
       </c>
-      <c r="F25" t="n">
-        <v>33.053827427644</v>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5.97629810979036</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="n">
-        <v>33.4167709637046</v>
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="n">
+        <v>8.59988171166419</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
       </c>
-      <c r="F27" t="n">
-        <v>28.3233532934132</v>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="n">
+        <v>4.69134156200255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" t="n">
-        <v>23.2356344003085</v>
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7.49949215009141</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
       </c>
-      <c r="F29" t="n">
-        <v>23.1912020065599</v>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="n">
+        <v>8.11214010305935</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" t="n">
-        <v>18.0403458213256</v>
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="n">
+        <v>15.6879978905819</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
       </c>
-      <c r="F31" t="n">
-        <v>24.0442579168256</v>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="n">
+        <v>11.1733113340966</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="n">
+        <v>6.90740090075702</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5.55285501328667</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="n">
+        <v>8.11791456354518</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6.20066344547153</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="n">
+        <v>5.28398379901824</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" t="n">
+        <v>4.65489868197319</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="n">
+        <v>7.04878409707493</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" t="n">
+        <v>4.11641988500483</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="n">
+        <v>4.57363336205516</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3.70498614958449</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="n">
+        <v>4.07999090614972</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3.37279565914416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>